<commit_message>
made it easier to copy over measures to the google doc
</commit_message>
<xml_diff>
--- a/Calculate Qualities.xlsx
+++ b/Calculate Qualities.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>DNA TP</t>
   </si>
@@ -126,19 +126,82 @@
   </si>
   <si>
     <t>Insert your values below</t>
+  </si>
+  <si>
+    <t>DNA Sensitivity</t>
+  </si>
+  <si>
+    <t>DNA specificity</t>
+  </si>
+  <si>
+    <t>DNA Predictive ACC</t>
+  </si>
+  <si>
+    <t>DNA MCC</t>
+  </si>
+  <si>
+    <t>RNA Sensitivity</t>
+  </si>
+  <si>
+    <t>RNA specificity</t>
+  </si>
+  <si>
+    <t>RNA Predictive ACC</t>
+  </si>
+  <si>
+    <t>RNA MCC</t>
+  </si>
+  <si>
+    <t>DRNA Sensitivity</t>
+  </si>
+  <si>
+    <t>DRNA specificity</t>
+  </si>
+  <si>
+    <t>DRNA Predictive ACC</t>
+  </si>
+  <si>
+    <t>DRNA MCC</t>
+  </si>
+  <si>
+    <t>nonDNA Sensitivity</t>
+  </si>
+  <si>
+    <t>nonDNA specificity</t>
+  </si>
+  <si>
+    <t>nonDNA Predictive ACC</t>
+  </si>
+  <si>
+    <t>nonDNA MCC</t>
+  </si>
+  <si>
+    <t>Copy the VALUES over to the google doc. Title the design with something descriptive (ie PAAC data using Random Forest)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -161,8 +224,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -615,52 +680,201 @@
         <v>25</v>
       </c>
     </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E11" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
+      <c r="D12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="e">
+        <f>E3</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
+      <c r="D13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="e">
+        <f>E4</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
+      <c r="D14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" t="e">
+        <f>E5</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" t="e">
+        <f>E6</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="e">
+        <f>F3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" t="e">
+        <f>F4</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" t="e">
+        <f>F5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" t="e">
+        <f>F6</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" t="e">
+        <f>G3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" t="e">
+        <f>G4</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>31</v>
       </c>
       <c r="B22">
         <v>8795</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="e">
+        <f>G5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" t="e">
+        <f>G6</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" t="e">
+        <f>H3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" t="e">
+        <f>H4</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" t="e">
+        <f>H5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" t="e">
+        <f>H6</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" t="e">
+        <f>E7</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29">
+        <f>E8</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>